<commit_message>
required vendor field of direct purchase in pr and jo
</commit_message>
<xml_diff>
--- a/uploads/format/pr form/PurchaseRequestFormcenpribcd.xlsx
+++ b/uploads/format/pr form/PurchaseRequestFormcenpribcd.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\purchasing\uploads\format\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\purchasing\uploads\format\pr form\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -446,71 +446,71 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -564,7 +564,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -864,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10:K10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,14 +891,14 @@
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="14"/>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
       <c r="I2" s="14"/>
       <c r="J2" s="14"/>
       <c r="K2" s="5"/>
@@ -906,14 +906,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="6"/>
@@ -921,14 +921,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="6"/>
@@ -936,58 +936,58 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="18"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="34"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="23"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="29"/>
       <c r="H7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="24"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="23"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="29"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="25" t="s">
+      <c r="B8" s="25"/>
+      <c r="C8" s="17" t="s">
         <v>64</v>
       </c>
       <c r="D8" s="26"/>
-      <c r="E8" s="27"/>
+      <c r="E8" s="18"/>
       <c r="H8" s="9" t="s">
         <v>62</v>
       </c>
@@ -998,64 +998,64 @@
       <c r="K8" s="39"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="25" t="s">
+      <c r="B9" s="25"/>
+      <c r="C9" s="17" t="s">
         <v>64</v>
       </c>
       <c r="D9" s="26"/>
-      <c r="E9" s="27"/>
+      <c r="E9" s="18"/>
       <c r="H9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="24"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="23"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="29"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="23"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="29"/>
       <c r="H10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="24"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="23"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="29"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="23"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="29"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="29"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="31"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="21"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -1070,169 +1070,142 @@
       <c r="D13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="32" t="s">
+      <c r="E13" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
       <c r="I13" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J13" s="32" t="s">
+      <c r="J13" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="33"/>
+      <c r="K13" s="23"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
       <c r="I14" s="10"/>
-      <c r="J14" s="25" t="s">
+      <c r="J14" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="K14" s="27"/>
+      <c r="K14" s="18"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
       <c r="I15" s="10"/>
-      <c r="J15" s="25" t="s">
+      <c r="J15" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="K15" s="27"/>
+      <c r="K15" s="18"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
       <c r="I16" s="10"/>
-      <c r="J16" s="25" t="s">
+      <c r="J16" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="K16" s="27"/>
+      <c r="K16" s="18"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
       <c r="I17" s="10"/>
-      <c r="J17" s="25" t="s">
+      <c r="J17" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="K17" s="27"/>
+      <c r="K17" s="18"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
       <c r="I18" s="10"/>
-      <c r="J18" s="25" t="s">
+      <c r="J18" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="K18" s="27"/>
+      <c r="K18" s="18"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
       <c r="I19" s="10"/>
-      <c r="J19" s="25" t="s">
+      <c r="J19" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="K19" s="27"/>
+      <c r="K19" s="18"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
       <c r="I20" s="10"/>
-      <c r="J20" s="25" t="s">
+      <c r="J20" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="K20" s="27"/>
+      <c r="K20" s="18"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
       <c r="I21" s="10"/>
-      <c r="J21" s="25" t="s">
+      <c r="J21" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="K21" s="27"/>
+      <c r="K21" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="E21:H21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="E18:H18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I9:K9"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
@@ -1243,6 +1216,33 @@
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="C7:E7"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="J20:K20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>